<commit_message>
Conclusao rodada 31 parte2
</commit_message>
<xml_diff>
--- a/dados/brasileirao2024_rodada26_38.xlsx
+++ b/dados/brasileirao2024_rodada26_38.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m4005001\Documents\_SG\Pessoal\Estatisticas_Brasileirao\estatisticas-brasileirao-masc\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD31930D-98A8-4ED3-BA89-926F62549E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE8C3FD-2980-4F57-A143-664411C2B652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{41E319D3-3B58-480D-98E9-32E41B6BA286}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{41E319D3-3B58-480D-98E9-32E41B6BA286}"/>
   </bookViews>
   <sheets>
     <sheet name="brasileirao2024_rodada26_38" sheetId="1" r:id="rId1"/>
@@ -1030,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F3D25C2-B42E-4952-80A2-82BCE65D805B}">
   <dimension ref="A1:F161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2825,6 +2825,12 @@
       <c r="D90" t="s">
         <v>18</v>
       </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90">
+        <v>1</v>
+      </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91">
@@ -2838,6 +2844,12 @@
       </c>
       <c r="D91" t="s">
         <v>23</v>
+      </c>
+      <c r="E91">
+        <v>3</v>
+      </c>
+      <c r="F91">
+        <v>2</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Rodada 33 - Aba projecoes
</commit_message>
<xml_diff>
--- a/dados/brasileirao2024_rodada26_38.xlsx
+++ b/dados/brasileirao2024_rodada26_38.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m4005001\Documents\_SG\Pessoal\Estatisticas_Brasileirao\estatisticas-brasileirao-masc\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE8C3FD-2980-4F57-A143-664411C2B652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0356EA4-AD74-488C-AFAB-A310FA1B3BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{41E319D3-3B58-480D-98E9-32E41B6BA286}"/>
+    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15990" xr2:uid="{41E319D3-3B58-480D-98E9-32E41B6BA286}"/>
   </bookViews>
   <sheets>
     <sheet name="brasileirao2024_rodada26_38" sheetId="1" r:id="rId1"/>
@@ -310,7 +310,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -490,6 +490,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -651,8 +657,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1030,8 +1037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F3D25C2-B42E-4952-80A2-82BCE65D805B}">
   <dimension ref="A1:F161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="F124" sqref="F124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1557,6 +1564,12 @@
       <c r="D26" t="s">
         <v>26</v>
       </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
@@ -1651,6 +1664,12 @@
       <c r="D31" t="s">
         <v>10</v>
       </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
@@ -2865,6 +2884,12 @@
       <c r="D92" t="s">
         <v>30</v>
       </c>
+      <c r="E92">
+        <v>2</v>
+      </c>
+      <c r="F92">
+        <v>2</v>
+      </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93">
@@ -2879,6 +2904,12 @@
       <c r="D93" t="s">
         <v>22</v>
       </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+      <c r="F93">
+        <v>0</v>
+      </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94">
@@ -2893,6 +2924,12 @@
       <c r="D94" t="s">
         <v>24</v>
       </c>
+      <c r="E94">
+        <v>1</v>
+      </c>
+      <c r="F94">
+        <v>2</v>
+      </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95">
@@ -2907,6 +2944,12 @@
       <c r="D95" t="s">
         <v>28</v>
       </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="F95">
+        <v>3</v>
+      </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96">
@@ -2921,8 +2964,14 @@
       <c r="D96" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E96">
+        <v>2</v>
+      </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>2024</v>
       </c>
@@ -2935,8 +2984,14 @@
       <c r="D97" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E97">
+        <v>1</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>2024</v>
       </c>
@@ -2949,8 +3004,14 @@
       <c r="D98" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E98">
+        <v>0</v>
+      </c>
+      <c r="F98">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>2024</v>
       </c>
@@ -2963,8 +3024,14 @@
       <c r="D99" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E99">
+        <v>3</v>
+      </c>
+      <c r="F99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>2024</v>
       </c>
@@ -2977,8 +3044,14 @@
       <c r="D100" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E100">
+        <v>0</v>
+      </c>
+      <c r="F100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>2024</v>
       </c>
@@ -2991,8 +3064,14 @@
       <c r="D101" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E101">
+        <v>1</v>
+      </c>
+      <c r="F101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>2024</v>
       </c>
@@ -3005,8 +3084,14 @@
       <c r="D102" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E102">
+        <v>2</v>
+      </c>
+      <c r="F102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>2024</v>
       </c>
@@ -3019,8 +3104,14 @@
       <c r="D103" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E103">
+        <v>1</v>
+      </c>
+      <c r="F103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>2024</v>
       </c>
@@ -3033,8 +3124,14 @@
       <c r="D104" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E104">
+        <v>1</v>
+      </c>
+      <c r="F104">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>2024</v>
       </c>
@@ -3047,8 +3144,14 @@
       <c r="D105" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E105">
+        <v>0</v>
+      </c>
+      <c r="F105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>2024</v>
       </c>
@@ -3061,8 +3164,14 @@
       <c r="D106" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E106">
+        <v>2</v>
+      </c>
+      <c r="F106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>2024</v>
       </c>
@@ -3075,8 +3184,14 @@
       <c r="D107" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E107">
+        <v>3</v>
+      </c>
+      <c r="F107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>2024</v>
       </c>
@@ -3089,8 +3204,14 @@
       <c r="D108" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E108">
+        <v>0</v>
+      </c>
+      <c r="F108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>2024</v>
       </c>
@@ -3103,8 +3224,14 @@
       <c r="D109" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E109">
+        <v>2</v>
+      </c>
+      <c r="F109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>2024</v>
       </c>
@@ -3117,8 +3244,14 @@
       <c r="D110" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E110">
+        <v>2</v>
+      </c>
+      <c r="F110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>2024</v>
       </c>
@@ -3131,8 +3264,14 @@
       <c r="D111" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E111">
+        <v>0</v>
+      </c>
+      <c r="F111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>2024</v>
       </c>
@@ -3145,8 +3284,14 @@
       <c r="D112" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E112">
+        <v>2</v>
+      </c>
+      <c r="F112">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>2024</v>
       </c>
@@ -3159,8 +3304,14 @@
       <c r="D113" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E113">
+        <v>0</v>
+      </c>
+      <c r="F113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>2024</v>
       </c>
@@ -3173,8 +3324,14 @@
       <c r="D114" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E114">
+        <v>1</v>
+      </c>
+      <c r="F114">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>2024</v>
       </c>
@@ -3187,8 +3344,10 @@
       <c r="D115" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E115" s="1"/>
+      <c r="F115" s="1"/>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>2024</v>
       </c>
@@ -3201,8 +3360,14 @@
       <c r="D116" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E116">
+        <v>0</v>
+      </c>
+      <c r="F116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>2024</v>
       </c>
@@ -3215,8 +3380,14 @@
       <c r="D117" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E117">
+        <v>2</v>
+      </c>
+      <c r="F117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>2024</v>
       </c>
@@ -3229,8 +3400,14 @@
       <c r="D118" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E118">
+        <v>1</v>
+      </c>
+      <c r="F118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>2024</v>
       </c>
@@ -3243,8 +3420,14 @@
       <c r="D119" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E119">
+        <v>2</v>
+      </c>
+      <c r="F119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>2024</v>
       </c>
@@ -3257,8 +3440,14 @@
       <c r="D120" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E120">
+        <v>1</v>
+      </c>
+      <c r="F120">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>2024</v>
       </c>
@@ -3271,8 +3460,14 @@
       <c r="D121" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E121">
+        <v>0</v>
+      </c>
+      <c r="F121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>2024</v>
       </c>
@@ -3286,7 +3481,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>2024</v>
       </c>
@@ -3300,7 +3495,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>2024</v>
       </c>
@@ -3314,7 +3509,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>2024</v>
       </c>
@@ -3328,7 +3523,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>2024</v>
       </c>
@@ -3342,7 +3537,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>2024</v>
       </c>
@@ -3356,7 +3551,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>2024</v>
       </c>

</xml_diff>

<commit_message>
Update - Rodada 38
</commit_message>
<xml_diff>
--- a/dados/brasileirao2024_rodada26_38.xlsx
+++ b/dados/brasileirao2024_rodada26_38.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m4005001\Documents\_SG\Pessoal\Estatisticas_Brasileirao\estatisticas-brasileirao-masc\dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m4005001\OneDrive - Saint-Gobain\Documents\_SG\Pessoal\Estatisticas_Brasileirao\estatisticas-brasileirao-masc\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD76CE68-6CC4-43D0-A0B8-3AC23511368D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2DE5C0-E7B5-4751-8888-566F90A6679D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="10340" xr2:uid="{41E319D3-3B58-480D-98E9-32E41B6BA286}"/>
+    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15990" xr2:uid="{41E319D3-3B58-480D-98E9-32E41B6BA286}"/>
   </bookViews>
   <sheets>
     <sheet name="brasileirao2024_rodada26_38" sheetId="1" r:id="rId1"/>
@@ -310,7 +310,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -490,12 +490,6 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -657,9 +651,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1037,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F3D25C2-B42E-4952-80A2-82BCE65D805B}">
   <dimension ref="A1:F161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B110" workbookViewId="0">
-      <selection activeCell="E132" sqref="E132"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H123" sqref="H123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3504,8 +3497,12 @@
       <c r="D123" t="s">
         <v>30</v>
       </c>
-      <c r="E123" s="1"/>
-      <c r="F123" s="1"/>
+      <c r="E123">
+        <v>1</v>
+      </c>
+      <c r="F123">
+        <v>1</v>
+      </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124">
@@ -3680,6 +3677,12 @@
       <c r="D132" t="s">
         <v>47</v>
       </c>
+      <c r="E132">
+        <v>2</v>
+      </c>
+      <c r="F132">
+        <v>1</v>
+      </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133">
@@ -3694,6 +3697,12 @@
       <c r="D133" t="s">
         <v>35</v>
       </c>
+      <c r="E133">
+        <v>2</v>
+      </c>
+      <c r="F133">
+        <v>3</v>
+      </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134">
@@ -3708,6 +3717,12 @@
       <c r="D134" t="s">
         <v>28</v>
       </c>
+      <c r="E134">
+        <v>2</v>
+      </c>
+      <c r="F134">
+        <v>0</v>
+      </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135">
@@ -3722,6 +3737,12 @@
       <c r="D135" t="s">
         <v>32</v>
       </c>
+      <c r="E135">
+        <v>3</v>
+      </c>
+      <c r="F135">
+        <v>2</v>
+      </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136">
@@ -3736,6 +3757,12 @@
       <c r="D136" t="s">
         <v>9</v>
       </c>
+      <c r="E136">
+        <v>2</v>
+      </c>
+      <c r="F136">
+        <v>2</v>
+      </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137">
@@ -3750,6 +3777,12 @@
       <c r="D137" t="s">
         <v>14</v>
       </c>
+      <c r="E137">
+        <v>1</v>
+      </c>
+      <c r="F137">
+        <v>3</v>
+      </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138">
@@ -3764,6 +3797,12 @@
       <c r="D138" t="s">
         <v>21</v>
       </c>
+      <c r="E138">
+        <v>1</v>
+      </c>
+      <c r="F138">
+        <v>1</v>
+      </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139">
@@ -3778,6 +3817,12 @@
       <c r="D139" t="s">
         <v>27</v>
       </c>
+      <c r="E139">
+        <v>1</v>
+      </c>
+      <c r="F139">
+        <v>1</v>
+      </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140">
@@ -3792,6 +3837,12 @@
       <c r="D140" t="s">
         <v>23</v>
       </c>
+      <c r="E140">
+        <v>1</v>
+      </c>
+      <c r="F140">
+        <v>2</v>
+      </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141">
@@ -3806,6 +3857,12 @@
       <c r="D141" t="s">
         <v>18</v>
       </c>
+      <c r="E141">
+        <v>2</v>
+      </c>
+      <c r="F141">
+        <v>4</v>
+      </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142">
@@ -3820,6 +3877,12 @@
       <c r="D142" t="s">
         <v>14</v>
       </c>
+      <c r="E142">
+        <v>0</v>
+      </c>
+      <c r="F142">
+        <v>1</v>
+      </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A143">
@@ -3834,6 +3897,12 @@
       <c r="D143" t="s">
         <v>37</v>
       </c>
+      <c r="E143">
+        <v>1</v>
+      </c>
+      <c r="F143">
+        <v>2</v>
+      </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144">
@@ -3848,8 +3917,14 @@
       <c r="D144" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E144">
+        <v>1</v>
+      </c>
+      <c r="F144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>2024</v>
       </c>
@@ -3862,8 +3937,14 @@
       <c r="D145" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E145">
+        <v>1</v>
+      </c>
+      <c r="F145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>2024</v>
       </c>
@@ -3876,8 +3957,14 @@
       <c r="D146" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E146">
+        <v>2</v>
+      </c>
+      <c r="F146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>2024</v>
       </c>
@@ -3890,8 +3977,14 @@
       <c r="D147" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E147">
+        <v>3</v>
+      </c>
+      <c r="F147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>2024</v>
       </c>
@@ -3904,8 +3997,14 @@
       <c r="D148" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E148">
+        <v>1</v>
+      </c>
+      <c r="F148">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>2024</v>
       </c>
@@ -3918,8 +4017,14 @@
       <c r="D149" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E149">
+        <v>1</v>
+      </c>
+      <c r="F149">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>2024</v>
       </c>
@@ -3932,8 +4037,14 @@
       <c r="D150" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E150">
+        <v>3</v>
+      </c>
+      <c r="F150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>2024</v>
       </c>
@@ -3946,8 +4057,14 @@
       <c r="D151" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E151">
+        <v>0</v>
+      </c>
+      <c r="F151">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>2024</v>
       </c>
@@ -3960,8 +4077,14 @@
       <c r="D152" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E152">
+        <v>0</v>
+      </c>
+      <c r="F152">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>2024</v>
       </c>
@@ -3974,8 +4097,14 @@
       <c r="D153" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E153">
+        <v>1</v>
+      </c>
+      <c r="F153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>2024</v>
       </c>
@@ -3988,8 +4117,14 @@
       <c r="D154" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E154">
+        <v>2</v>
+      </c>
+      <c r="F154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>2024</v>
       </c>
@@ -4002,8 +4137,14 @@
       <c r="D155" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E155">
+        <v>2</v>
+      </c>
+      <c r="F155">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>2024</v>
       </c>
@@ -4016,8 +4157,14 @@
       <c r="D156" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E156">
+        <v>2</v>
+      </c>
+      <c r="F156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>2024</v>
       </c>
@@ -4030,8 +4177,14 @@
       <c r="D157" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E157">
+        <v>0</v>
+      </c>
+      <c r="F157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>2024</v>
       </c>
@@ -4044,8 +4197,14 @@
       <c r="D158" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E158">
+        <v>5</v>
+      </c>
+      <c r="F158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>2024</v>
       </c>
@@ -4058,8 +4217,14 @@
       <c r="D159" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E159">
+        <v>3</v>
+      </c>
+      <c r="F159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>2024</v>
       </c>
@@ -4072,8 +4237,14 @@
       <c r="D160" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E160">
+        <v>1</v>
+      </c>
+      <c r="F160">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>2024</v>
       </c>
@@ -4085,6 +4256,12 @@
       </c>
       <c r="D161" t="s">
         <v>21</v>
+      </c>
+      <c r="E161">
+        <v>0</v>
+      </c>
+      <c r="F161">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update - Comparativos - de selectobx para multiselect
</commit_message>
<xml_diff>
--- a/dados/brasileirao2024_rodada26_38.xlsx
+++ b/dados/brasileirao2024_rodada26_38.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m4005001\OneDrive - Saint-Gobain\Documents\_SG\Pessoal\Estatisticas_Brasileirao\estatisticas-brasileirao-masc\dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://saintgobain-my.sharepoint.com/personal/mario_deus_saint-gobain_com/Documents/Pessoal/Estatisticas_Brasileirao/estatisticas-brasileirao-masc/dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2DE5C0-E7B5-4751-8888-566F90A6679D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{5F2DE5C0-E7B5-4751-8888-566F90A6679D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1DA5146-BACE-4CF3-B32E-A327268B32FC}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15990" xr2:uid="{41E319D3-3B58-480D-98E9-32E41B6BA286}"/>
   </bookViews>
@@ -1030,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F3D25C2-B42E-4952-80A2-82BCE65D805B}">
   <dimension ref="A1:F161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H123" sqref="H123"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="N86" sqref="N86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2978,7 +2978,7 @@
         <v>20</v>
       </c>
       <c r="E97">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F97">
         <v>0</v>
@@ -3001,7 +3001,7 @@
         <v>0</v>
       </c>
       <c r="F98">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>